<commit_message>
Definities afrekenwijze en bestedingsoort
</commit_message>
<xml_diff>
--- a/Referentiedata/VERA - Referentiedata - 2022-07-08.xlsx
+++ b/Referentiedata/VERA - Referentiedata - 2022-07-08.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewout\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewout\Documents\GitHub\VERA-Standaard\Referentiedata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77CE576E-9606-4C65-9291-297769B3089A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7915915E-8A50-4DF6-8F6D-AC63E431A430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14332,8 +14332,8 @@
   <dimension ref="A1:K1373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1197" sqref="A1197"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51525,6 +51525,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFD438D9B9ABE14A977C2E01E1E997E9" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="238b4f00df057bc2742cc7aff66473ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="41b44f4d-acd5-45c0-8ca7-9032ca64d707" xmlns:ns3="bc2bfcf0-0204-42b7-916d-bc08fc5e6372" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfb8db5c6f5549a83cd0326992bdc891" ns2:_="" ns3:_="">
     <xsd:import namespace="41b44f4d-acd5-45c0-8ca7-9032ca64d707"/>
@@ -51727,15 +51736,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E3AA29B-E85A-4662-AF70-E41EEBB4502A}">
   <ds:schemaRefs>
@@ -51746,6 +51746,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9FCA9DB-B654-4D97-A1BC-1B4528FD4E25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -51762,12 +51770,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update VERA - Referentiedata - 2022-07-08.xlsx
Toelichting ruimtesoort zolder
</commit_message>
<xml_diff>
--- a/Referentiedata/VERA - Referentiedata - 2022-07-08.xlsx
+++ b/Referentiedata/VERA - Referentiedata - 2022-07-08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VERA\VERA-Standaard\Referentiedata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2693569-BE5E-4590-B094-0A54D4611F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C115EAC6-71E8-421C-8504-98788E1FFD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3771" yWindow="3771" windowWidth="24686" windowHeight="13106" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13158,9 +13158,6 @@
     <t>De onderhoudsorder wordt afgerekend op basis van aantal eenheden x eenheidsrpijs. Bij bestedingsoort kan hier gebruik gemaakt worden van de soort Vaste taakprijs</t>
   </si>
   <si>
-    <t>Overige ruimte; is de bovenste verdieping direct onder het dak van een gebouw met een vaste trap zoals gedefinieerd voor het bepalen van de woningwaardering. De term wordt vooral gebruikt bij gebouwen met een puntdak. De bovenste verdieping van een gebouw met plat dak wordt meestal geen zolder genoemd.</t>
-  </si>
-  <si>
     <t>ZAAKROL</t>
   </si>
   <si>
@@ -13228,6 +13225,9 @@
   </si>
   <si>
     <t>EINDEREDEN.ONT</t>
+  </si>
+  <si>
+    <t>Overige ruimte; is de bovenste verdieping direct onder het dak van een gebouw met een vaste trap zoals gedefinieerd voor het bepalen van de woningwaardering. De term wordt vooral gebruikt bij gebouwen met een puntdak. De bovenste verdieping van een gebouw met plat dak wordt meestal geen zolder genoemd. Een ruimte mag als vertrek worden gezien indien deze een vast trap heeft, de vloer begaanbaar en het dak beschoten is. Zolders zonder vaste trap leggen we niet vast als vertrek. Indien een woning een zolder heeft met een vlizotrap kan dit in de advertentietekst worden gemeld.</t>
   </si>
 </sst>
 </file>
@@ -14026,8 +14026,7 @@
   <autoFilter ref="A1:K1385" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}">
     <filterColumn colId="0">
       <filters>
-        <filter val="EINDEDETAILREDEN"/>
-        <filter val="EINDEREDEN"/>
+        <filter val="RUIMTESOORT"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -14408,8 +14407,8 @@
   <dimension ref="A1:K1385"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A577" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H583" sqref="H583"/>
+      <pane ySplit="1" topLeftCell="A1199" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1213" sqref="E1213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -27401,7 +27400,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="577" spans="1:11" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="577" spans="1:11" s="10" customFormat="1" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A577" s="10" t="s">
         <v>4132</v>
       </c>
@@ -27417,13 +27416,13 @@
       <c r="F577" s="11"/>
       <c r="G577" s="11"/>
       <c r="H577" s="10" t="s">
-        <v>4341</v>
+        <v>4340</v>
       </c>
       <c r="I577" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="578" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="578" spans="1:11" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A578" s="10" t="s">
         <v>4132</v>
       </c>
@@ -27439,13 +27438,13 @@
       <c r="F578" s="11"/>
       <c r="G578" s="11"/>
       <c r="H578" s="10" t="s">
-        <v>4342</v>
+        <v>4341</v>
       </c>
       <c r="I578" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="579" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="579" spans="1:11" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A579" s="10" t="s">
         <v>4132</v>
       </c>
@@ -27461,13 +27460,13 @@
       <c r="F579" s="11"/>
       <c r="G579" s="11"/>
       <c r="H579" s="10" t="s">
-        <v>4342</v>
+        <v>4341</v>
       </c>
       <c r="I579" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="580" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="580" spans="1:11" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A580" s="10" t="s">
         <v>4132</v>
       </c>
@@ -27483,13 +27482,13 @@
       <c r="F580" s="11"/>
       <c r="G580" s="11"/>
       <c r="H580" s="10" t="s">
-        <v>4342</v>
+        <v>4341</v>
       </c>
       <c r="I580" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="581" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="581" spans="1:11" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A581" s="10" t="s">
         <v>4132</v>
       </c>
@@ -27505,13 +27504,13 @@
       <c r="F581" s="11"/>
       <c r="G581" s="11"/>
       <c r="H581" s="10" t="s">
-        <v>4342</v>
+        <v>4341</v>
       </c>
       <c r="I581" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="582" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="582" spans="1:11" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A582" s="10" t="s">
         <v>4132</v>
       </c>
@@ -27527,13 +27526,13 @@
       <c r="F582" s="11"/>
       <c r="G582" s="11"/>
       <c r="H582" s="10" t="s">
-        <v>4341</v>
+        <v>4340</v>
       </c>
       <c r="I582" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="583" spans="1:11" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="583" spans="1:11" s="10" customFormat="1" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A583" s="10" t="s">
         <v>4132</v>
       </c>
@@ -27549,13 +27548,13 @@
       <c r="F583" s="11"/>
       <c r="G583" s="11"/>
       <c r="H583" s="10" t="s">
-        <v>4341</v>
+        <v>4340</v>
       </c>
       <c r="I583" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="584" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="584" spans="1:11" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A584" s="10" t="s">
         <v>4132</v>
       </c>
@@ -27571,13 +27570,13 @@
       <c r="F584" s="11"/>
       <c r="G584" s="11"/>
       <c r="H584" s="10" t="s">
-        <v>4341</v>
+        <v>4340</v>
       </c>
       <c r="I584" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="585" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="585" spans="1:11" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A585" s="10" t="s">
         <v>4132</v>
       </c>
@@ -27593,13 +27592,13 @@
       <c r="F585" s="11"/>
       <c r="G585" s="11"/>
       <c r="H585" s="10" t="s">
-        <v>4341</v>
+        <v>4340</v>
       </c>
       <c r="I585" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="586" spans="1:11" s="10" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="586" spans="1:11" s="10" customFormat="1" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
       <c r="A586" s="10" t="s">
         <v>3913</v>
       </c>
@@ -27618,7 +27617,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="587" spans="1:11" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="587" spans="1:11" s="10" customFormat="1" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A587" s="10" t="s">
         <v>3913</v>
       </c>
@@ -27637,7 +27636,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="588" spans="1:11" s="10" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="588" spans="1:11" s="10" customFormat="1" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
       <c r="A588" s="10" t="s">
         <v>3913</v>
       </c>
@@ -40988,7 +40987,7 @@
       <c r="J1189" s="14"/>
       <c r="K1189" s="14"/>
     </row>
-    <row r="1190" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1190" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1190" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41011,7 +41010,7 @@
       <c r="J1190" s="13"/>
       <c r="K1190" s="13"/>
     </row>
-    <row r="1191" spans="1:11" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1191" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A1191" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41034,7 +41033,7 @@
       <c r="J1191" s="13"/>
       <c r="K1191" s="13"/>
     </row>
-    <row r="1192" spans="1:11" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1192" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A1192" s="13" t="s">
         <v>1911</v>
       </c>
@@ -41057,7 +41056,7 @@
       <c r="J1192" s="13"/>
       <c r="K1192" s="13"/>
     </row>
-    <row r="1193" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1193" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1193" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41080,7 +41079,7 @@
       <c r="J1193" s="13"/>
       <c r="K1193" s="13"/>
     </row>
-    <row r="1194" spans="1:11" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1194" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A1194" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41103,7 +41102,7 @@
       <c r="J1194" s="13"/>
       <c r="K1194" s="13"/>
     </row>
-    <row r="1195" spans="1:11" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1195" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A1195" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41126,7 +41125,7 @@
       <c r="J1195" s="13"/>
       <c r="K1195" s="13"/>
     </row>
-    <row r="1196" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1196" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1196" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41149,7 +41148,7 @@
       <c r="J1196" s="13"/>
       <c r="K1196" s="13"/>
     </row>
-    <row r="1197" spans="1:11" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1197" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A1197" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41172,7 +41171,7 @@
       <c r="J1197" s="13"/>
       <c r="K1197" s="13"/>
     </row>
-    <row r="1198" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1198" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1198" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41195,7 +41194,7 @@
       <c r="J1198" s="13"/>
       <c r="K1198" s="13"/>
     </row>
-    <row r="1199" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1199" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1199" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41218,7 +41217,7 @@
       <c r="J1199" s="13"/>
       <c r="K1199" s="13"/>
     </row>
-    <row r="1200" spans="1:11" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1200" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A1200" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41241,7 +41240,7 @@
       <c r="J1200" s="13"/>
       <c r="K1200" s="13"/>
     </row>
-    <row r="1201" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1201" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1201" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41264,7 +41263,7 @@
       <c r="J1201" s="13"/>
       <c r="K1201" s="13"/>
     </row>
-    <row r="1202" spans="1:11" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1202" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A1202" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41287,7 +41286,7 @@
       <c r="J1202" s="13"/>
       <c r="K1202" s="13"/>
     </row>
-    <row r="1203" spans="1:11" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1203" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A1203" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41310,7 +41309,7 @@
       <c r="J1203" s="13"/>
       <c r="K1203" s="13"/>
     </row>
-    <row r="1204" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1204" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1204" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41331,7 +41330,7 @@
       <c r="J1204" s="10"/>
       <c r="K1204" s="10"/>
     </row>
-    <row r="1205" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1205" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1205" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41354,7 +41353,7 @@
       <c r="J1205" s="13"/>
       <c r="K1205" s="13"/>
     </row>
-    <row r="1206" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1206" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1206" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41377,7 +41376,7 @@
       <c r="J1206" s="13"/>
       <c r="K1206" s="13"/>
     </row>
-    <row r="1207" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1207" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1207" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41398,7 +41397,7 @@
       <c r="J1207" s="10"/>
       <c r="K1207" s="10"/>
     </row>
-    <row r="1208" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1208" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1208" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41421,7 +41420,7 @@
       <c r="J1208" s="13"/>
       <c r="K1208" s="13"/>
     </row>
-    <row r="1209" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1209" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1209" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41444,7 +41443,7 @@
       <c r="J1209" s="10"/>
       <c r="K1209" s="10"/>
     </row>
-    <row r="1210" spans="1:11" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1210" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A1210" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41467,7 +41466,7 @@
       <c r="J1210" s="13"/>
       <c r="K1210" s="13"/>
     </row>
-    <row r="1211" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1211" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1211" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41488,7 +41487,7 @@
       <c r="J1211" s="10"/>
       <c r="K1211" s="10"/>
     </row>
-    <row r="1212" spans="1:11" ht="58.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1212" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A1212" s="36" t="s">
         <v>1911</v>
       </c>
@@ -41500,7 +41499,7 @@
         <v>1929</v>
       </c>
       <c r="E1212" s="12" t="s">
-        <v>4319</v>
+        <v>4342</v>
       </c>
       <c r="F1212" s="12"/>
       <c r="G1212" s="12"/>
@@ -41511,7 +41510,7 @@
       <c r="J1212" s="13"/>
       <c r="K1212" s="13"/>
     </row>
-    <row r="1213" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
+    <row r="1213" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1213" s="25" t="s">
         <v>1911</v>
       </c>
@@ -45382,14 +45381,14 @@
     </row>
     <row r="1374" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1374" s="10" t="s">
-        <v>4320</v>
+        <v>4319</v>
       </c>
       <c r="B1374" s="10"/>
       <c r="C1374" s="10" t="s">
         <v>1117</v>
       </c>
       <c r="D1374" s="11" t="s">
-        <v>4321</v>
+        <v>4320</v>
       </c>
       <c r="E1374" s="11"/>
       <c r="F1374" s="11"/>
@@ -45401,7 +45400,7 @@
     </row>
     <row r="1375" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1375" s="10" t="s">
-        <v>4320</v>
+        <v>4319</v>
       </c>
       <c r="B1375" s="10"/>
       <c r="C1375" s="10" t="s">
@@ -45420,14 +45419,14 @@
     </row>
     <row r="1376" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1376" s="10" t="s">
-        <v>4320</v>
+        <v>4319</v>
       </c>
       <c r="B1376" s="10"/>
       <c r="C1376" s="10" t="s">
-        <v>4327</v>
+        <v>4326</v>
       </c>
       <c r="D1376" s="11" t="s">
-        <v>4322</v>
+        <v>4321</v>
       </c>
       <c r="E1376" s="11"/>
       <c r="F1376" s="11"/>
@@ -45439,14 +45438,14 @@
     </row>
     <row r="1377" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1377" s="10" t="s">
-        <v>4320</v>
+        <v>4319</v>
       </c>
       <c r="B1377" s="10"/>
       <c r="C1377" s="10" t="s">
         <v>916</v>
       </c>
       <c r="D1377" s="11" t="s">
-        <v>4323</v>
+        <v>4322</v>
       </c>
       <c r="E1377" s="11"/>
       <c r="F1377" s="11"/>
@@ -45458,14 +45457,14 @@
     </row>
     <row r="1378" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1378" s="10" t="s">
-        <v>4320</v>
+        <v>4319</v>
       </c>
       <c r="B1378" s="10"/>
       <c r="C1378" s="10" t="s">
-        <v>4328</v>
+        <v>4327</v>
       </c>
       <c r="D1378" s="11" t="s">
-        <v>4324</v>
+        <v>4323</v>
       </c>
       <c r="E1378" s="11"/>
       <c r="F1378" s="11"/>
@@ -45477,14 +45476,14 @@
     </row>
     <row r="1379" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1379" s="10" t="s">
-        <v>4320</v>
+        <v>4319</v>
       </c>
       <c r="B1379" s="10"/>
       <c r="C1379" s="10" t="s">
         <v>1880</v>
       </c>
       <c r="D1379" s="11" t="s">
-        <v>4326</v>
+        <v>4325</v>
       </c>
       <c r="E1379" s="11"/>
       <c r="F1379" s="11"/>
@@ -45496,14 +45495,14 @@
     </row>
     <row r="1380" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1380" s="10" t="s">
-        <v>4320</v>
+        <v>4319</v>
       </c>
       <c r="B1380" s="10"/>
       <c r="C1380" s="10" t="s">
-        <v>4329</v>
+        <v>4328</v>
       </c>
       <c r="D1380" s="11" t="s">
-        <v>4325</v>
+        <v>4324</v>
       </c>
       <c r="E1380" s="11"/>
       <c r="F1380" s="11"/>
@@ -45515,14 +45514,14 @@
     </row>
     <row r="1381" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1381" s="10" t="s">
-        <v>4330</v>
+        <v>4329</v>
       </c>
       <c r="B1381" s="10"/>
       <c r="C1381" s="10" t="s">
-        <v>4331</v>
+        <v>4330</v>
       </c>
       <c r="D1381" s="11" t="s">
-        <v>4336</v>
+        <v>4335</v>
       </c>
       <c r="E1381" s="11"/>
       <c r="F1381" s="11"/>
@@ -45534,14 +45533,14 @@
     </row>
     <row r="1382" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1382" s="10" t="s">
-        <v>4330</v>
+        <v>4329</v>
       </c>
       <c r="B1382" s="10"/>
       <c r="C1382" s="10" t="s">
-        <v>4332</v>
+        <v>4331</v>
       </c>
       <c r="D1382" s="11" t="s">
-        <v>4337</v>
+        <v>4336</v>
       </c>
       <c r="E1382" s="11"/>
       <c r="F1382" s="11"/>
@@ -45553,14 +45552,14 @@
     </row>
     <row r="1383" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1383" s="10" t="s">
-        <v>4330</v>
+        <v>4329</v>
       </c>
       <c r="B1383" s="10"/>
       <c r="C1383" s="10" t="s">
-        <v>4333</v>
+        <v>4332</v>
       </c>
       <c r="D1383" s="11" t="s">
-        <v>4338</v>
+        <v>4337</v>
       </c>
       <c r="E1383" s="11"/>
       <c r="F1383" s="11"/>
@@ -45572,14 +45571,14 @@
     </row>
     <row r="1384" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1384" s="10" t="s">
-        <v>4330</v>
+        <v>4329</v>
       </c>
       <c r="B1384" s="10"/>
       <c r="C1384" s="10" t="s">
-        <v>4334</v>
+        <v>4333</v>
       </c>
       <c r="D1384" s="11" t="s">
-        <v>4339</v>
+        <v>4338</v>
       </c>
       <c r="E1384" s="11"/>
       <c r="F1384" s="11"/>
@@ -45591,14 +45590,14 @@
     </row>
     <row r="1385" spans="1:11" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1385" s="10" t="s">
-        <v>4330</v>
+        <v>4329</v>
       </c>
       <c r="B1385" s="10"/>
       <c r="C1385" s="10" t="s">
-        <v>4335</v>
+        <v>4334</v>
       </c>
       <c r="D1385" s="11" t="s">
-        <v>4340</v>
+        <v>4339</v>
       </c>
       <c r="E1385" s="11"/>
       <c r="F1385" s="11"/>
@@ -51856,15 +51855,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFD438D9B9ABE14A977C2E01E1E997E9" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="238b4f00df057bc2742cc7aff66473ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="41b44f4d-acd5-45c0-8ca7-9032ca64d707" xmlns:ns3="bc2bfcf0-0204-42b7-916d-bc08fc5e6372" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfb8db5c6f5549a83cd0326992bdc891" ns2:_="" ns3:_="">
     <xsd:import namespace="41b44f4d-acd5-45c0-8ca7-9032ca64d707"/>
@@ -52067,6 +52057,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E3AA29B-E85A-4662-AF70-E41EEBB4502A}">
   <ds:schemaRefs>
@@ -52077,14 +52076,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9FCA9DB-B654-4D97-A1BC-1B4528FD4E25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -52101,4 +52092,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>